<commit_message>
DB Backup - Stake and cus position
</commit_message>
<xml_diff>
--- a/SVS-IMPORT-UPDATEPROJECT.xlsx
+++ b/SVS-IMPORT-UPDATEPROJECT.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86F5F15-6944-43D6-9CFC-F956FCD62D59}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC457515-28D8-43E3-938B-ACA093144DFF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25875" yWindow="3120" windowWidth="20115" windowHeight="9930" tabRatio="686" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="4275" windowWidth="20115" windowHeight="9930" tabRatio="686" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="project_info" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Laguna, Calabarzon, Philippines</t>
   </si>
@@ -69,12 +69,6 @@
     <t>2019-1004</t>
   </si>
   <si>
-    <t>2019-1003</t>
-  </si>
-  <si>
-    <t>2019-1002</t>
-  </si>
-  <si>
     <t>pm_member_code</t>
   </si>
   <si>
@@ -109,6 +103,15 @@
   </si>
   <si>
     <t>target_man_days</t>
+  </si>
+  <si>
+    <t>2020-C7DVWDZ7</t>
+  </si>
+  <si>
+    <t>2019-UIDMS</t>
+  </si>
+  <si>
+    <t>2020-JH9UHG26</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6F89B1-F1C8-4F81-AFF8-898276C7AC65}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -489,7 +492,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -513,18 +516,18 @@
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="2">
         <v>43770.128472222219</v>
@@ -584,7 +587,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +602,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -622,7 +625,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -639,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF74F18C-FC59-48AF-B173-EFF79CAD16CB}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,17 +653,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -686,21 +689,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>50</v>

</xml_diff>